<commit_message>
se agregan datos del anuario 2019 para OOSS y huelgas
</commit_message>
<xml_diff>
--- a/Output/Cuadros/1. OOSS/cuadro1.xlsx
+++ b/Output/Cuadros/1. OOSS/cuadro1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1316,6 +1316,38 @@
         <v>20.6</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31">
+        <v>2019</v>
+      </c>
+      <c r="B31">
+        <v>11926</v>
+      </c>
+      <c r="C31">
+        <v>1193104</v>
+      </c>
+      <c r="D31">
+        <v>9107664.122137405</v>
+      </c>
+      <c r="E31">
+        <v>13.1</v>
+      </c>
+      <c r="F31">
+        <v>7503798.742138364</v>
+      </c>
+      <c r="G31">
+        <v>15.9</v>
+      </c>
+      <c r="H31">
+        <v>1066996</v>
+      </c>
+      <c r="I31">
+        <v>5645481.481481481</v>
+      </c>
+      <c r="J31">
+        <v>18.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>